<commit_message>
Fix NCES ids of school districts in ME file. Another one.
</commit_message>
<xml_diff>
--- a/data/nces_lookups/ME_schools_nces_lookup.xlsx
+++ b/data/nces_lookups/ME_schools_nces_lookup.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="1288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="1286">
   <si>
     <t>SchoolName</t>
   </si>
@@ -2914,12 +2914,6 @@
   </si>
   <si>
     <t>RSU #21 School District</t>
-  </si>
-  <si>
-    <t>000002314773</t>
-  </si>
-  <si>
-    <t>0000023</t>
   </si>
   <si>
     <t>Ralph M Atwood Primary School</t>
@@ -8769,19 +8763,16 @@
       <c r="A420" s="2" t="s">
         <v>965</v>
       </c>
-      <c r="B420" s="2" t="s">
-        <v>966</v>
-      </c>
-      <c r="C420" s="2" t="s">
-        <v>967</v>
+      <c r="C420" s="4" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="421" ht="15.75" customHeight="1">
       <c r="A421" s="2" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="B421" s="2" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>72</v>
@@ -8789,21 +8780,21 @@
     </row>
     <row r="422" ht="15.75" customHeight="1">
       <c r="A422" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="B422" s="2" t="s">
+        <v>969</v>
+      </c>
+      <c r="C422" s="2" t="s">
         <v>970</v>
-      </c>
-      <c r="B422" s="2" t="s">
-        <v>971</v>
-      </c>
-      <c r="C422" s="2" t="s">
-        <v>972</v>
       </c>
     </row>
     <row r="423" ht="15.75" customHeight="1">
       <c r="A423" s="2" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="B423" s="2" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="C423" s="2" t="s">
         <v>390</v>
@@ -8811,10 +8802,10 @@
     </row>
     <row r="424" ht="15.75" customHeight="1">
       <c r="A424" s="2" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="B424" s="2" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="C424" s="2" t="s">
         <v>390</v>
@@ -8822,10 +8813,10 @@
     </row>
     <row r="425" ht="15.75" customHeight="1">
       <c r="A425" s="2" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="B425" s="2" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="C425" s="2" t="s">
         <v>585</v>
@@ -8833,10 +8824,10 @@
     </row>
     <row r="426" ht="15.75" customHeight="1">
       <c r="A426" s="2" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="C426" s="2" t="s">
         <v>718</v>
@@ -8844,10 +8835,10 @@
     </row>
     <row r="427" ht="15.75" customHeight="1">
       <c r="A427" s="2" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="B427" s="2" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="C427" s="2" t="s">
         <v>313</v>
@@ -8855,18 +8846,18 @@
     </row>
     <row r="428" ht="15.75" customHeight="1">
       <c r="A428" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="B428" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="C428" s="2" t="s">
         <v>982</v>
-      </c>
-      <c r="B428" s="2" t="s">
-        <v>983</v>
-      </c>
-      <c r="C428" s="2" t="s">
-        <v>984</v>
       </c>
     </row>
     <row r="429" ht="15.75" customHeight="1">
       <c r="A429" s="2" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="B429" s="2" t="s">
         <v>556</v>
@@ -8877,10 +8868,10 @@
     </row>
     <row r="430" ht="15.75" customHeight="1">
       <c r="A430" s="2" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="B430" s="2" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="C430" s="2" t="s">
         <v>304</v>
@@ -8888,10 +8879,10 @@
     </row>
     <row r="431" ht="15.75" customHeight="1">
       <c r="A431" s="2" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="B431" s="2" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>304</v>
@@ -8899,10 +8890,10 @@
     </row>
     <row r="432" ht="15.75" customHeight="1">
       <c r="A432" s="2" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="B432" s="2" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>281</v>
@@ -8910,10 +8901,10 @@
     </row>
     <row r="433" ht="15.75" customHeight="1">
       <c r="A433" s="2" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="B433" s="2" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>434</v>
@@ -8921,10 +8912,10 @@
     </row>
     <row r="434" ht="15.75" customHeight="1">
       <c r="A434" s="2" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B434" s="2" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>390</v>
@@ -8932,10 +8923,10 @@
     </row>
     <row r="435" ht="15.75" customHeight="1">
       <c r="A435" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="B435" s="2" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C435" s="2" t="s">
         <v>390</v>
@@ -8943,10 +8934,10 @@
     </row>
     <row r="436" ht="15.75" customHeight="1">
       <c r="A436" s="2" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>390</v>
@@ -8954,10 +8945,10 @@
     </row>
     <row r="437" ht="15.75" customHeight="1">
       <c r="A437" s="2" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="B437" s="2" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="C437" s="2" t="s">
         <v>545</v>
@@ -8965,10 +8956,10 @@
     </row>
     <row r="438" ht="15.75" customHeight="1">
       <c r="A438" s="2" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="B438" s="2" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>684</v>
@@ -8976,10 +8967,10 @@
     </row>
     <row r="439" ht="15.75" customHeight="1">
       <c r="A439" s="2" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="B439" s="2" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>684</v>
@@ -8987,10 +8978,10 @@
     </row>
     <row r="440" ht="15.75" customHeight="1">
       <c r="A440" s="2" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B440" s="2" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C440" s="2" t="s">
         <v>684</v>
@@ -8998,10 +8989,10 @@
     </row>
     <row r="441" ht="15.75" customHeight="1">
       <c r="A441" s="2" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="B441" s="2" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C441" s="2" t="s">
         <v>684</v>
@@ -9009,10 +9000,10 @@
     </row>
     <row r="442" ht="15.75" customHeight="1">
       <c r="A442" s="2" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="B442" s="2" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C442" s="2" t="s">
         <v>684</v>
@@ -9020,7 +9011,7 @@
     </row>
     <row r="443" ht="15.75" customHeight="1">
       <c r="A443" s="2" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="B443" s="2" t="s">
         <v>34</v>
@@ -9031,10 +9022,10 @@
     </row>
     <row r="444" ht="15.75" customHeight="1">
       <c r="A444" s="2" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="B444" s="2" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C444" s="2" t="s">
         <v>136</v>
@@ -9042,10 +9033,10 @@
     </row>
     <row r="445" ht="15.75" customHeight="1">
       <c r="A445" s="2" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="B445" s="2" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="C445" s="2" t="s">
         <v>144</v>
@@ -9053,7 +9044,7 @@
     </row>
     <row r="446" ht="15.75" customHeight="1">
       <c r="A446" s="2" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B446" s="2" t="s">
         <v>143</v>
@@ -9064,10 +9055,10 @@
     </row>
     <row r="447" ht="15.75" customHeight="1">
       <c r="A447" s="2" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B447" s="2" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="C447" s="2" t="s">
         <v>197</v>
@@ -9075,10 +9066,10 @@
     </row>
     <row r="448" ht="15.75" customHeight="1">
       <c r="A448" s="2" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="B448" s="2" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C448" s="2" t="s">
         <v>244</v>
@@ -9086,10 +9077,10 @@
     </row>
     <row r="449" ht="15.75" customHeight="1">
       <c r="A449" s="2" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="B449" s="2" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C449" s="2" t="s">
         <v>149</v>
@@ -9097,10 +9088,10 @@
     </row>
     <row r="450" ht="15.75" customHeight="1">
       <c r="A450" s="2" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="B450" s="2" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="C450" s="2" t="s">
         <v>149</v>
@@ -9108,65 +9099,65 @@
     </row>
     <row r="451" ht="15.75" customHeight="1">
       <c r="A451" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B451" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C451" s="2" t="s">
         <v>1020</v>
-      </c>
-      <c r="B451" s="2" t="s">
-        <v>1021</v>
-      </c>
-      <c r="C451" s="2" t="s">
-        <v>1022</v>
       </c>
     </row>
     <row r="452" ht="15.75" customHeight="1">
       <c r="A452" s="2" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="B452" s="2" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C452" s="2" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="453" ht="15.75" customHeight="1">
       <c r="A453" s="2" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="B453" s="2" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C453" s="2" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="454" ht="15.75" customHeight="1">
       <c r="A454" s="2" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="B454" s="2" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C454" s="2" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="455" ht="15.75" customHeight="1">
       <c r="A455" s="2" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B455" s="2" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C455" s="2" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="456" ht="15.75" customHeight="1">
       <c r="A456" s="2" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B456" s="2" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C456" s="2" t="s">
         <v>313</v>
@@ -9174,10 +9165,10 @@
     </row>
     <row r="457" ht="15.75" customHeight="1">
       <c r="A457" s="2" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="B457" s="2" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C457" s="2" t="s">
         <v>187</v>
@@ -9185,10 +9176,10 @@
     </row>
     <row r="458" ht="15.75" customHeight="1">
       <c r="A458" s="2" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C458" s="2" t="s">
         <v>187</v>
@@ -9196,10 +9187,10 @@
     </row>
     <row r="459" ht="15.75" customHeight="1">
       <c r="A459" s="2" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B459" s="2" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="C459" s="2" t="s">
         <v>187</v>
@@ -9207,10 +9198,10 @@
     </row>
     <row r="460" ht="15.75" customHeight="1">
       <c r="A460" s="2" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C460" s="2" t="s">
         <v>95</v>
@@ -9218,10 +9209,10 @@
     </row>
     <row r="461" ht="15.75" customHeight="1">
       <c r="A461" s="2" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="C461" s="2" t="s">
         <v>95</v>
@@ -9229,10 +9220,10 @@
     </row>
     <row r="462" ht="15.75" customHeight="1">
       <c r="A462" s="2" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="C462" s="2" t="s">
         <v>884</v>
@@ -9240,32 +9231,32 @@
     </row>
     <row r="463" ht="15.75" customHeight="1">
       <c r="A463" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B463" s="2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C463" s="2" t="s">
         <v>1043</v>
-      </c>
-      <c r="B463" s="2" t="s">
-        <v>1044</v>
-      </c>
-      <c r="C463" s="2" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="464" ht="15.75" customHeight="1">
       <c r="A464" s="2" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="C464" s="2" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="465" ht="15.75" customHeight="1">
       <c r="A465" s="2" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="B465" s="2" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="C465" s="2" t="s">
         <v>595</v>
@@ -9273,54 +9264,54 @@
     </row>
     <row r="466" ht="15.75" customHeight="1">
       <c r="A466" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B466" s="2" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C466" s="2" t="s">
         <v>1050</v>
-      </c>
-      <c r="B466" s="2" t="s">
-        <v>1051</v>
-      </c>
-      <c r="C466" s="2" t="s">
-        <v>1052</v>
       </c>
     </row>
     <row r="467" ht="15.75" customHeight="1">
       <c r="A467" s="2" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="B467" s="2" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="C467" s="2" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="468" ht="15.75" customHeight="1">
       <c r="A468" s="2" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="B468" s="2" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="C468" s="2" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="469" ht="15.75" customHeight="1">
       <c r="A469" s="2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B469" s="2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C469" s="2" t="s">
         <v>1057</v>
-      </c>
-      <c r="B469" s="2" t="s">
-        <v>1058</v>
-      </c>
-      <c r="C469" s="2" t="s">
-        <v>1059</v>
       </c>
     </row>
     <row r="470" ht="15.75" customHeight="1">
       <c r="A470" s="2" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="B470" s="2" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="C470" s="2" t="s">
         <v>368</v>
@@ -9328,10 +9319,10 @@
     </row>
     <row r="471" ht="15.75" customHeight="1">
       <c r="A471" s="2" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="B471" s="2" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="C471" s="2" t="s">
         <v>32</v>
@@ -9339,7 +9330,7 @@
     </row>
     <row r="472" ht="15.75" customHeight="1">
       <c r="A472" s="2" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="B472" s="2" t="s">
         <v>562</v>
@@ -9350,10 +9341,10 @@
     </row>
     <row r="473" ht="15.75" customHeight="1">
       <c r="A473" s="2" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="B473" s="2" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C473" s="2" t="s">
         <v>323</v>
@@ -9361,10 +9352,10 @@
     </row>
     <row r="474" ht="15.75" customHeight="1">
       <c r="A474" s="2" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="B474" s="2" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="C474" s="2" t="s">
         <v>53</v>
@@ -9372,10 +9363,10 @@
     </row>
     <row r="475" ht="15.75" customHeight="1">
       <c r="A475" s="2" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="B475" s="2" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="C475" s="2" t="s">
         <v>53</v>
@@ -9383,10 +9374,10 @@
     </row>
     <row r="476" ht="15.75" customHeight="1">
       <c r="A476" s="2" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="C476" s="2" t="s">
         <v>293</v>
@@ -9394,10 +9385,10 @@
     </row>
     <row r="477" ht="15.75" customHeight="1">
       <c r="A477" s="2" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="B477" s="2" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="C477" s="2" t="s">
         <v>89</v>
@@ -9405,10 +9396,10 @@
     </row>
     <row r="478" ht="15.75" customHeight="1">
       <c r="A478" s="2" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="B478" s="2" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="C478" s="2" t="s">
         <v>89</v>
@@ -9416,10 +9407,10 @@
     </row>
     <row r="479" ht="15.75" customHeight="1">
       <c r="A479" s="2" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="B479" s="2" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="C479" s="2" t="s">
         <v>89</v>
@@ -9427,10 +9418,10 @@
     </row>
     <row r="480" ht="15.75" customHeight="1">
       <c r="A480" s="2" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="B480" s="2" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="C480" s="2" t="s">
         <v>89</v>
@@ -9438,21 +9429,21 @@
     </row>
     <row r="481" ht="15.75" customHeight="1">
       <c r="A481" s="2" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B481" s="2" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C481" s="2" t="s">
         <v>1078</v>
-      </c>
-      <c r="B481" s="2" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C481" s="2" t="s">
-        <v>1080</v>
       </c>
     </row>
     <row r="482" ht="15.75" customHeight="1">
       <c r="A482" s="2" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="B482" s="2" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="C482" s="2" t="s">
         <v>368</v>
@@ -9460,10 +9451,10 @@
     </row>
     <row r="483" ht="15.75" customHeight="1">
       <c r="A483" s="2" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="B483" s="2" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C483" s="2" t="s">
         <v>611</v>
@@ -9471,10 +9462,10 @@
     </row>
     <row r="484" ht="15.75" customHeight="1">
       <c r="A484" s="2" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="B484" s="2" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="C484" s="2" t="s">
         <v>293</v>
@@ -9482,10 +9473,10 @@
     </row>
     <row r="485" ht="15.75" customHeight="1">
       <c r="A485" s="2" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="B485" s="2" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="C485" s="2" t="s">
         <v>47</v>
@@ -9493,76 +9484,76 @@
     </row>
     <row r="486" ht="15.75" customHeight="1">
       <c r="A486" s="2" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="C486" s="2" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="487" ht="15.75" customHeight="1">
       <c r="A487" s="2" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B487" s="2" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C487" s="2" t="s">
         <v>1090</v>
-      </c>
-      <c r="B487" s="2" t="s">
-        <v>1091</v>
-      </c>
-      <c r="C487" s="2" t="s">
-        <v>1092</v>
       </c>
     </row>
     <row r="488" ht="15.75" customHeight="1">
       <c r="A488" s="2" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="B488" s="2" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="C488" s="2" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="489" ht="15.75" customHeight="1">
       <c r="A489" s="2" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="B489" s="2" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="C489" s="2" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="490" ht="15.75" customHeight="1">
       <c r="A490" s="2" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="C490" s="2" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="491" ht="15.75" customHeight="1">
       <c r="A491" s="2" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B491" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C491" s="2" t="s">
         <v>1099</v>
-      </c>
-      <c r="B491" s="2" t="s">
-        <v>1100</v>
-      </c>
-      <c r="C491" s="2" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="492" ht="15.75" customHeight="1">
       <c r="A492" s="2" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="B492" s="2" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="C492" s="2" t="s">
         <v>461</v>
@@ -9570,10 +9561,10 @@
     </row>
     <row r="493" ht="15.75" customHeight="1">
       <c r="A493" s="2" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="B493" s="2" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="C493" s="2" t="s">
         <v>98</v>
@@ -9581,10 +9572,10 @@
     </row>
     <row r="494" ht="15.75" customHeight="1">
       <c r="A494" s="2" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="B494" s="2" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="C494" s="2" t="s">
         <v>611</v>
@@ -9592,21 +9583,21 @@
     </row>
     <row r="495" ht="15.75" customHeight="1">
       <c r="A495" s="2" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B495" s="2" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C495" s="2" t="s">
         <v>1108</v>
-      </c>
-      <c r="B495" s="2" t="s">
-        <v>1109</v>
-      </c>
-      <c r="C495" s="2" t="s">
-        <v>1110</v>
       </c>
     </row>
     <row r="496" ht="15.75" customHeight="1">
       <c r="A496" s="2" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="B496" s="2" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C496" s="2" t="s">
         <v>606</v>
@@ -9614,10 +9605,10 @@
     </row>
     <row r="497" ht="15.75" customHeight="1">
       <c r="A497" s="2" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C497" s="2" t="s">
         <v>204</v>
@@ -9625,10 +9616,10 @@
     </row>
     <row r="498" ht="15.75" customHeight="1">
       <c r="A498" s="2" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="B498" s="2" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C498" s="2" t="s">
         <v>177</v>
@@ -9636,10 +9627,10 @@
     </row>
     <row r="499" ht="15.75" customHeight="1">
       <c r="A499" s="2" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="B499" s="2" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C499" s="2" t="s">
         <v>253</v>
@@ -9647,10 +9638,10 @@
     </row>
     <row r="500" ht="15.75" customHeight="1">
       <c r="A500" s="2" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="B500" s="2" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C500" s="2" t="s">
         <v>253</v>
@@ -9658,7 +9649,7 @@
     </row>
     <row r="501" ht="15.75" customHeight="1">
       <c r="A501" s="2" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="B501" s="2" t="s">
         <v>290</v>
@@ -9669,10 +9660,10 @@
     </row>
     <row r="502" ht="15.75" customHeight="1">
       <c r="A502" s="2" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="B502" s="2" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="C502" s="2" t="s">
         <v>258</v>
@@ -9680,10 +9671,10 @@
     </row>
     <row r="503" ht="15.75" customHeight="1">
       <c r="A503" s="2" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="B503" s="2" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="C503" s="2" t="s">
         <v>258</v>
@@ -9691,7 +9682,7 @@
     </row>
     <row r="504" ht="15.75" customHeight="1">
       <c r="A504" s="2" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="B504" s="2" t="s">
         <v>753</v>
@@ -9702,10 +9693,10 @@
     </row>
     <row r="505" ht="15.75" customHeight="1">
       <c r="A505" s="2" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="B505" s="2" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="C505" s="2" t="s">
         <v>47</v>
@@ -9713,32 +9704,32 @@
     </row>
     <row r="506" ht="15.75" customHeight="1">
       <c r="A506" s="2" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B506" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C506" s="2" t="s">
         <v>1128</v>
-      </c>
-      <c r="B506" s="2" t="s">
-        <v>1129</v>
-      </c>
-      <c r="C506" s="2" t="s">
-        <v>1130</v>
       </c>
     </row>
     <row r="507" ht="15.75" customHeight="1">
       <c r="A507" s="2" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B507" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C507" s="2" t="s">
         <v>1131</v>
-      </c>
-      <c r="B507" s="2" t="s">
-        <v>1132</v>
-      </c>
-      <c r="C507" s="2" t="s">
-        <v>1133</v>
       </c>
     </row>
     <row r="508" ht="15.75" customHeight="1">
       <c r="A508" s="2" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="B508" s="2" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C508" s="2" t="s">
         <v>281</v>
@@ -9746,10 +9737,10 @@
     </row>
     <row r="509" ht="15.75" customHeight="1">
       <c r="A509" s="2" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="B509" s="2" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C509" s="2" t="s">
         <v>480</v>
@@ -9757,10 +9748,10 @@
     </row>
     <row r="510" ht="15.75" customHeight="1">
       <c r="A510" s="2" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="B510" s="2" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="C510" s="2" t="s">
         <v>38</v>
@@ -9768,10 +9759,10 @@
     </row>
     <row r="511" ht="15.75" customHeight="1">
       <c r="A511" s="2" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="B511" s="2" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="C511" s="2" t="s">
         <v>832</v>
@@ -9779,10 +9770,10 @@
     </row>
     <row r="512" ht="15.75" customHeight="1">
       <c r="A512" s="2" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="B512" s="2" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="C512" s="2" t="s">
         <v>832</v>
@@ -9790,10 +9781,10 @@
     </row>
     <row r="513" ht="15.75" customHeight="1">
       <c r="A513" s="2" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="B513" s="2" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="C513" s="2" t="s">
         <v>480</v>
@@ -9801,10 +9792,10 @@
     </row>
     <row r="514" ht="15.75" customHeight="1">
       <c r="A514" s="2" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="B514" s="2" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="C514" s="2" t="s">
         <v>480</v>
@@ -9812,10 +9803,10 @@
     </row>
     <row r="515" ht="15.75" customHeight="1">
       <c r="A515" s="2" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="B515" s="2" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C515" s="2" t="s">
         <v>427</v>
@@ -9823,21 +9814,21 @@
     </row>
     <row r="516" ht="15.75" customHeight="1">
       <c r="A516" s="2" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B516" s="2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C516" s="2" t="s">
         <v>1149</v>
-      </c>
-      <c r="B516" s="2" t="s">
-        <v>1150</v>
-      </c>
-      <c r="C516" s="2" t="s">
-        <v>1151</v>
       </c>
     </row>
     <row r="517" ht="15.75" customHeight="1">
       <c r="A517" s="2" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="B517" s="2" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="C517" s="2" t="s">
         <v>808</v>
@@ -9845,10 +9836,10 @@
     </row>
     <row r="518" ht="15.75" customHeight="1">
       <c r="A518" s="2" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="B518" s="2" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="C518" s="2" t="s">
         <v>406</v>
@@ -9856,10 +9847,10 @@
     </row>
     <row r="519" ht="15.75" customHeight="1">
       <c r="A519" s="2" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="B519" s="2" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="C519" s="2" t="s">
         <v>676</v>
@@ -9867,43 +9858,43 @@
     </row>
     <row r="520" ht="15.75" customHeight="1">
       <c r="A520" s="2" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B520" s="2" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C520" s="2" t="s">
         <v>1158</v>
-      </c>
-      <c r="B520" s="2" t="s">
-        <v>1159</v>
-      </c>
-      <c r="C520" s="2" t="s">
-        <v>1160</v>
       </c>
     </row>
     <row r="521" ht="15.75" customHeight="1">
       <c r="A521" s="2" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B521" s="2" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C521" s="2" t="s">
         <v>1161</v>
-      </c>
-      <c r="B521" s="2" t="s">
-        <v>1162</v>
-      </c>
-      <c r="C521" s="2" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="522" ht="15.75" customHeight="1">
       <c r="A522" s="2" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B522" s="2" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C522" s="2" t="s">
         <v>1164</v>
-      </c>
-      <c r="B522" s="2" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C522" s="2" t="s">
-        <v>1166</v>
       </c>
     </row>
     <row r="523" ht="15.75" customHeight="1">
       <c r="A523" s="2" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="B523" s="2" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="C523" s="2" t="s">
         <v>454</v>
@@ -9911,10 +9902,10 @@
     </row>
     <row r="524" ht="15.75" customHeight="1">
       <c r="A524" s="2" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="B524" s="2" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="C524" s="2" t="s">
         <v>238</v>
@@ -9922,10 +9913,10 @@
     </row>
     <row r="525" ht="15.75" customHeight="1">
       <c r="A525" s="2" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="B525" s="2" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="C525" s="2" t="s">
         <v>8</v>
@@ -9933,10 +9924,10 @@
     </row>
     <row r="526" ht="15.75" customHeight="1">
       <c r="A526" s="2" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="B526" s="2" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="C526" s="2" t="s">
         <v>365</v>
@@ -9944,7 +9935,7 @@
     </row>
     <row r="527" ht="15.75" customHeight="1">
       <c r="A527" s="2" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="B527" s="2" t="s">
         <v>715</v>
@@ -9955,21 +9946,21 @@
     </row>
     <row r="528" ht="15.75" customHeight="1">
       <c r="A528" s="2" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B528" s="2" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C528" s="2" t="s">
         <v>1176</v>
-      </c>
-      <c r="B528" s="2" t="s">
-        <v>1177</v>
-      </c>
-      <c r="C528" s="2" t="s">
-        <v>1178</v>
       </c>
     </row>
     <row r="529" ht="15.75" customHeight="1">
       <c r="A529" s="2" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="B529" s="2" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="C529" s="2" t="s">
         <v>293</v>
@@ -9977,10 +9968,10 @@
     </row>
     <row r="530" ht="15.75" customHeight="1">
       <c r="A530" s="2" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="B530" s="2" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C530" s="2" t="s">
         <v>53</v>
@@ -9988,10 +9979,10 @@
     </row>
     <row r="531" ht="15.75" customHeight="1">
       <c r="A531" s="2" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="B531" s="2" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C531" s="2" t="s">
         <v>427</v>
@@ -9999,43 +9990,43 @@
     </row>
     <row r="532" ht="15.75" customHeight="1">
       <c r="A532" s="2" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="B532" s="2" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C532" s="2" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="533" ht="15.75" customHeight="1">
       <c r="A533" s="2" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B533" s="2" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C533" s="2" t="s">
         <v>1186</v>
-      </c>
-      <c r="B533" s="2" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C533" s="2" t="s">
-        <v>1188</v>
       </c>
     </row>
     <row r="534" ht="15.75" customHeight="1">
       <c r="A534" s="2" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="B534" s="2" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="C534" s="2" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="535" ht="15.75" customHeight="1">
       <c r="A535" s="2" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B535" s="2" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="C535" s="2" t="s">
         <v>53</v>
@@ -10043,10 +10034,10 @@
     </row>
     <row r="536" ht="15.75" customHeight="1">
       <c r="A536" s="2" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="B536" s="2" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="C536" s="2" t="s">
         <v>32</v>
@@ -10054,10 +10045,10 @@
     </row>
     <row r="537" ht="15.75" customHeight="1">
       <c r="A537" s="2" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="B537" s="2" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="C537" s="2" t="s">
         <v>23</v>
@@ -10065,10 +10056,10 @@
     </row>
     <row r="538" ht="15.75" customHeight="1">
       <c r="A538" s="2" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="B538" s="2" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="C538" s="2" t="s">
         <v>26</v>
@@ -10076,10 +10067,10 @@
     </row>
     <row r="539" ht="15.75" customHeight="1">
       <c r="A539" s="2" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="B539" s="2" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="C539" s="2" t="s">
         <v>26</v>
@@ -10087,10 +10078,10 @@
     </row>
     <row r="540" ht="15.75" customHeight="1">
       <c r="A540" s="2" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="B540" s="2" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="C540" s="2" t="s">
         <v>718</v>
@@ -10098,43 +10089,43 @@
     </row>
     <row r="541" ht="15.75" customHeight="1">
       <c r="A541" s="2" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B541" s="2" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C541" s="2" t="s">
         <v>1202</v>
-      </c>
-      <c r="B541" s="2" t="s">
-        <v>1203</v>
-      </c>
-      <c r="C541" s="2" t="s">
-        <v>1204</v>
       </c>
     </row>
     <row r="542" ht="15.75" customHeight="1">
       <c r="A542" s="2" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="B542" s="2" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="C542" s="2" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="543" ht="15.75" customHeight="1">
       <c r="A543" s="2" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="B543" s="2" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C543" s="2" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="544" ht="15.75" customHeight="1">
       <c r="A544" s="2" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="B544" s="2" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="C544" s="2" t="s">
         <v>95</v>
@@ -10142,21 +10133,21 @@
     </row>
     <row r="545" ht="15.75" customHeight="1">
       <c r="A545" s="2" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B545" s="2" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C545" s="2" t="s">
         <v>1211</v>
-      </c>
-      <c r="B545" s="2" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C545" s="2" t="s">
-        <v>1213</v>
       </c>
     </row>
     <row r="546" ht="15.75" customHeight="1">
       <c r="A546" s="2" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="B546" s="2" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="C546" s="2" t="s">
         <v>244</v>
@@ -10164,10 +10155,10 @@
     </row>
     <row r="547" ht="15.75" customHeight="1">
       <c r="A547" s="2" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="B547" s="2" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="C547" s="2" t="s">
         <v>244</v>
@@ -10175,10 +10166,10 @@
     </row>
     <row r="548" ht="15.75" customHeight="1">
       <c r="A548" s="2" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="B548" s="2" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="C548" s="2" t="s">
         <v>244</v>
@@ -10186,10 +10177,10 @@
     </row>
     <row r="549" ht="15.75" customHeight="1">
       <c r="A549" s="2" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="B549" s="2" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="C549" s="2" t="s">
         <v>244</v>
@@ -10197,10 +10188,10 @@
     </row>
     <row r="550" ht="15.75" customHeight="1">
       <c r="A550" s="2" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="B550" s="2" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="C550" s="2" t="s">
         <v>226</v>
@@ -10208,10 +10199,10 @@
     </row>
     <row r="551" ht="15.75" customHeight="1">
       <c r="A551" s="2" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="B551" s="2" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="C551" s="2" t="s">
         <v>187</v>
@@ -10219,10 +10210,10 @@
     </row>
     <row r="552" ht="15.75" customHeight="1">
       <c r="A552" s="2" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="B552" s="2" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="C552" s="2" t="s">
         <v>418</v>
@@ -10230,10 +10221,10 @@
     </row>
     <row r="553" ht="15.75" customHeight="1">
       <c r="A553" s="2" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="B553" s="2" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="C553" s="2" t="s">
         <v>8</v>
@@ -10241,10 +10232,10 @@
     </row>
     <row r="554" ht="15.75" customHeight="1">
       <c r="A554" s="2" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="B554" s="2" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="C554" s="2" t="s">
         <v>72</v>
@@ -10252,10 +10243,10 @@
     </row>
     <row r="555" ht="15.75" customHeight="1">
       <c r="A555" s="2" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="B555" s="2" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="C555" s="2" t="s">
         <v>108</v>
@@ -10263,10 +10254,10 @@
     </row>
     <row r="556" ht="15.75" customHeight="1">
       <c r="A556" s="2" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="B556" s="2" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="C556" s="2" t="s">
         <v>585</v>
@@ -10274,10 +10265,10 @@
     </row>
     <row r="557" ht="15.75" customHeight="1">
       <c r="A557" s="2" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="B557" s="2" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="C557" s="2" t="s">
         <v>585</v>
@@ -10285,10 +10276,10 @@
     </row>
     <row r="558" ht="15.75" customHeight="1">
       <c r="A558" s="2" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="B558" s="2" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="C558" s="2" t="s">
         <v>585</v>
@@ -10296,10 +10287,10 @@
     </row>
     <row r="559" ht="15.75" customHeight="1">
       <c r="A559" s="2" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B559" s="2" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="C559" s="2" t="s">
         <v>226</v>
@@ -10307,98 +10298,98 @@
     </row>
     <row r="560" ht="15.75" customHeight="1">
       <c r="A560" s="2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B560" s="2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C560" s="2" t="s">
         <v>1242</v>
-      </c>
-      <c r="B560" s="2" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C560" s="2" t="s">
-        <v>1244</v>
       </c>
     </row>
     <row r="561" ht="15.75" customHeight="1">
       <c r="A561" s="2" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="B561" s="2" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="C561" s="2" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="562" ht="15.75" customHeight="1">
       <c r="A562" s="2" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="B562" s="2" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="C562" s="2" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="563" ht="15.75" customHeight="1">
       <c r="A563" s="2" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B563" s="2" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C563" s="2" t="s">
         <v>1249</v>
-      </c>
-      <c r="B563" s="2" t="s">
-        <v>1250</v>
-      </c>
-      <c r="C563" s="2" t="s">
-        <v>1251</v>
       </c>
     </row>
     <row r="564" ht="15.75" customHeight="1">
       <c r="A564" s="2" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="B564" s="2" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="C564" s="2" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="565" ht="15.75" customHeight="1">
       <c r="A565" s="2" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="B565" s="2" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="C565" s="2" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="566" ht="15.75" customHeight="1">
       <c r="A566" s="2" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B566" s="2" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C566" s="2" t="s">
         <v>1256</v>
-      </c>
-      <c r="B566" s="2" t="s">
-        <v>1257</v>
-      </c>
-      <c r="C566" s="2" t="s">
-        <v>1258</v>
       </c>
     </row>
     <row r="567" ht="15.75" customHeight="1">
       <c r="A567" s="2" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="B567" s="2" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="C567" s="2" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="568" ht="15.75" customHeight="1">
       <c r="A568" s="2" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="B568" s="2" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="C568" s="2" t="s">
         <v>298</v>
@@ -10406,43 +10397,43 @@
     </row>
     <row r="569" ht="15.75" customHeight="1">
       <c r="A569" s="2" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B569" s="2" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C569" s="2" t="s">
         <v>1263</v>
-      </c>
-      <c r="B569" s="2" t="s">
-        <v>1264</v>
-      </c>
-      <c r="C569" s="2" t="s">
-        <v>1265</v>
       </c>
     </row>
     <row r="570" ht="15.75" customHeight="1">
       <c r="A570" s="2" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B570" s="2" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C570" s="2" t="s">
         <v>1266</v>
-      </c>
-      <c r="B570" s="2" t="s">
-        <v>1267</v>
-      </c>
-      <c r="C570" s="2" t="s">
-        <v>1268</v>
       </c>
     </row>
     <row r="571" ht="15.75" customHeight="1">
       <c r="A571" s="2" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="B571" s="2" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="C571" s="2" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="572" ht="15.75" customHeight="1">
       <c r="A572" s="2" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="B572" s="2" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="C572" s="2" t="s">
         <v>108</v>
@@ -10450,10 +10441,10 @@
     </row>
     <row r="573" ht="15.75" customHeight="1">
       <c r="A573" s="2" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="B573" s="2" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="C573" s="2" t="s">
         <v>258</v>
@@ -10461,10 +10452,10 @@
     </row>
     <row r="574" ht="15.75" customHeight="1">
       <c r="A574" s="2" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="B574" s="2" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="C574" s="2" t="s">
         <v>58</v>
@@ -10472,10 +10463,10 @@
     </row>
     <row r="575" ht="15.75" customHeight="1">
       <c r="A575" s="2" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="B575" s="2" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="C575" s="2" t="s">
         <v>418</v>
@@ -10483,10 +10474,10 @@
     </row>
     <row r="576" ht="15.75" customHeight="1">
       <c r="A576" s="2" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="B576" s="2" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="C576" s="2" t="s">
         <v>418</v>
@@ -10494,10 +10485,10 @@
     </row>
     <row r="577" ht="15.75" customHeight="1">
       <c r="A577" s="2" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="B577" s="2" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="C577" s="2" t="s">
         <v>238</v>
@@ -10505,10 +10496,10 @@
     </row>
     <row r="578" ht="15.75" customHeight="1">
       <c r="A578" s="2" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="B578" s="2" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="C578" s="2" t="s">
         <v>238</v>
@@ -10516,10 +10507,10 @@
     </row>
     <row r="579" ht="15.75" customHeight="1">
       <c r="A579" s="2" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="B579" s="2" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="C579" s="2" t="s">
         <v>149</v>
@@ -10527,7 +10518,7 @@
     </row>
     <row r="580" ht="15.75" customHeight="1">
       <c r="A580" s="2" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="B580" s="2" t="s">
         <v>370</v>

</xml_diff>